<commit_message>
Added .ods file support and added events for additional customization.
</commit_message>
<xml_diff>
--- a/samples/8_special_template/exported_file.xlsx
+++ b/samples/8_special_template/exported_file.xlsx
@@ -25,7 +25,7 @@
     <t>*подробнее уточняйте у менеджеров магазина.</t>
   </si>
   <si>
-    <t>Бланк заказа №1111111 от 2018-11-06</t>
+    <t>Бланк заказа №1111111 от 2019-10-02</t>
   </si>
   <si>
     <t>Заказчик</t>
@@ -170,7 +170,7 @@
     <t>(подпись исполнителя)</t>
   </si>
   <si>
-    <t>Квитанция к заказу №1111111 от 2018-11-06</t>
+    <t>Квитанция к заказу №1111111 от 2019-10-02</t>
   </si>
   <si>
     <t>{auto}</t>

</xml_diff>